<commit_message>
fix jframe dimensions so shows pppwd
</commit_message>
<xml_diff>
--- a/records/permanentRecord_Alice Brown.xlsx
+++ b/records/permanentRecord_Alice Brown.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Date and Time</t>
   </si>
@@ -45,52 +45,49 @@
     <t>Level</t>
   </si>
   <si>
-    <t>2026-01-13 01:19:16</t>
-  </si>
-  <si>
-    <t>RespRate</t>
-  </si>
-  <si>
-    <t>11.0 - 11.0</t>
+    <t>2026-01-13 21:35:05</t>
+  </si>
+  <si>
+    <t>ECG</t>
+  </si>
+  <si>
+    <t>-0.9 - -0.9</t>
   </si>
   <si>
     <t>AMBER</t>
   </si>
   <si>
-    <t>2026-01-13 01:19:17</t>
-  </si>
-  <si>
-    <t>ECG</t>
-  </si>
-  <si>
-    <t>1.0 - 1.0</t>
+    <t>2026-01-13 21:35:12</t>
+  </si>
+  <si>
+    <t>-0.8 - -0.8</t>
+  </si>
+  <si>
+    <t>2026-01-13 21:35:16</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>35.1 - 35.9</t>
+  </si>
+  <si>
+    <t>2026-01-13 21:35:19</t>
+  </si>
+  <si>
+    <t>0.9 - 0.9</t>
   </si>
   <si>
     <t>RED</t>
   </si>
   <si>
-    <t>2026-01-13 01:19:19</t>
-  </si>
-  <si>
-    <t>-0.8 - -0.8</t>
-  </si>
-  <si>
-    <t>2026-01-13 01:19:18</t>
-  </si>
-  <si>
-    <t>2026-01-13 01:19:21</t>
-  </si>
-  <si>
-    <t>10.0 - 11.0</t>
-  </si>
-  <si>
-    <t>2026-01-13 01:19:22</t>
-  </si>
-  <si>
-    <t>2026-01-13 01:19:23</t>
-  </si>
-  <si>
-    <t>0.7 - 0.9</t>
+    <t>2026-01-13 21:35:20</t>
+  </si>
+  <si>
+    <t>2026-01-13 21:35:21</t>
+  </si>
+  <si>
+    <t>-0.9 - -0.8</t>
   </si>
 </sst>
 </file>
@@ -213,27 +210,27 @@
         <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>16</v>
-      </c>
       <c r="E3" t="s" s="0">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>18</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>19</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>13</v>
@@ -241,33 +238,33 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="E5" t="s" s="0">
         <v>21</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="C6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>24</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>25</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>13</v>

</xml_diff>

<commit_message>
comment heartbeat + unit test patient
</commit_message>
<xml_diff>
--- a/records/permanentRecord_Alice Brown.xlsx
+++ b/records/permanentRecord_Alice Brown.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Date and Time</t>
   </si>
@@ -45,49 +45,31 @@
     <t>Level</t>
   </si>
   <si>
-    <t>2026-01-13 21:35:05</t>
+    <t>2026-01-14 01:42:56</t>
   </si>
   <si>
     <t>ECG</t>
   </si>
   <si>
-    <t>-0.9 - -0.9</t>
+    <t>0.9 - 0.9</t>
   </si>
   <si>
     <t>AMBER</t>
   </si>
   <si>
-    <t>2026-01-13 21:35:12</t>
-  </si>
-  <si>
-    <t>-0.8 - -0.8</t>
-  </si>
-  <si>
-    <t>2026-01-13 21:35:16</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>35.1 - 35.9</t>
-  </si>
-  <si>
-    <t>2026-01-13 21:35:19</t>
-  </si>
-  <si>
-    <t>0.9 - 0.9</t>
+    <t>2026-01-14 01:42</t>
+  </si>
+  <si>
+    <t>112/85</t>
+  </si>
+  <si>
+    <t>2026-01-14 01:43:03</t>
+  </si>
+  <si>
+    <t>-1.0 - -1.0</t>
   </si>
   <si>
     <t>RED</t>
-  </si>
-  <si>
-    <t>2026-01-13 21:35:20</t>
-  </si>
-  <si>
-    <t>2026-01-13 21:35:21</t>
-  </si>
-  <si>
-    <t>-0.9 - -0.8</t>
   </si>
 </sst>
 </file>
@@ -132,7 +114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -155,6 +137,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>71.0</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -162,7 +161,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -204,70 +203,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s" s="0">
         <v>18</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>